<commit_message>
Modified parsing of CSV/XLS spreadsheets in DOIInputUtil to ignore the status column and support parsing of several optional columns
</commit_message>
<xml_diff>
--- a/input/DOI_Reserved_GEO_200318_with_invalid_rows.xlsx
+++ b/input/DOI_Reserved_GEO_200318_with_invalid_rows.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/collinss/repos/pds-doi-service/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34E7D240-3783-9946-A4FA-A641FC47C7A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEB938FE-1B1E-9445-A6E3-BC5C1972B4EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
-  <si>
-    <t>status</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>title</t>
   </si>
@@ -43,9 +40,6 @@
     <t>related_resource</t>
   </si>
   <si>
-    <t>Reserved</t>
-  </si>
-  <si>
     <t>Laboratory Shocked Feldspars Bundle</t>
   </si>
   <si>
@@ -76,16 +70,10 @@
     <t>J3. R3.</t>
   </si>
   <si>
-    <t>urn:nasa:pds:lab_shocked_feldspars::11.0</t>
-  </si>
-  <si>
     <t>urn:nasa:pds:lab_shocked_feldspars_21::1.0</t>
   </si>
   <si>
     <t>urn:nasa:pds:lab_shocked_feldspars_31::1.0</t>
-  </si>
-  <si>
-    <t>Alright</t>
   </si>
   <si>
     <t>invalid_date</t>
@@ -451,20 +439,20 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="33.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="38.33203125" customWidth="1"/>
-    <col min="8" max="8" width="22.1640625" customWidth="1"/>
+    <col min="1" max="1" width="33.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="38.33203125" customWidth="1"/>
+    <col min="7" max="7" width="22.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -483,80 +471,66 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="2">
+        <v>43901</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="1"/>
+      <c r="B3" s="2">
+        <v>43902</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1"/>
-    </row>
-    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="2">
-        <v>43901</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="B4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" s="1"/>
-    </row>
-    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="2">
-        <v>43902</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="1"/>
-    </row>
-    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H4" s="1"/>
+      <c r="G4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>